<commit_message>
left with chemo regimen
</commit_message>
<xml_diff>
--- a/input/input variables sheet.xlsx
+++ b/input/input variables sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\programming\clinical_research\ovarian_chemo\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EFB82D-9724-4B78-9927-380116592BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE279306-55A8-423C-B5EE-78D27B407D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-160" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{037ECBA2-1291-EA4D-8C7B-C557A09F4A75}"/>
+    <workbookView xWindow="-38510" yWindow="-160" windowWidth="19420" windowHeight="11020" xr2:uid="{037ECBA2-1291-EA4D-8C7B-C557A09F4A75}"/>
   </bookViews>
   <sheets>
     <sheet name="Group 2" sheetId="1" r:id="rId1"/>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AD70A9-FE78-594E-B7B8-BA08F5EC3010}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9772F212-CF78-E842-A07E-47783236D83E}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView topLeftCell="C5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L25" sqref="L24:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>

</xml_diff>